<commit_message>
added util function to fetch name of the applicant
</commit_message>
<xml_diff>
--- a/cvscan/data/job_positions/positions.xlsx
+++ b/cvscan/data/job_positions/positions.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="jobs_summary" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2092" uniqueCount="716">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2089" uniqueCount="715">
   <si>
     <t xml:space="preserve">Job Title</t>
   </si>
@@ -1226,9 +1226,6 @@
   </si>
   <si>
     <t xml:space="preserve">founder owner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hr</t>
   </si>
   <si>
     <t xml:space="preserve">hr generalist</t>
@@ -2346,17 +2343,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D697"/>
+  <dimension ref="A1:D696"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A299" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A390" activeCellId="0" sqref="A390"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.5991902834008"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="19.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="27.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8038,7 +8035,7 @@
         <v>3</v>
       </c>
       <c r="C406" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D406" s="1" t="s">
         <v>13</v>
@@ -8220,7 +8217,7 @@
         <v>3</v>
       </c>
       <c r="C419" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D419" s="1" t="s">
         <v>13</v>
@@ -8402,7 +8399,7 @@
         <v>3</v>
       </c>
       <c r="C432" s="1" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
       <c r="D432" s="1" t="s">
         <v>13</v>
@@ -8416,7 +8413,7 @@
         <v>3</v>
       </c>
       <c r="C433" s="1" t="s">
-        <v>118</v>
+        <v>5</v>
       </c>
       <c r="D433" s="1" t="s">
         <v>13</v>
@@ -8469,10 +8466,10 @@
         <v>449</v>
       </c>
       <c r="B437" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C437" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D437" s="1" t="s">
         <v>13</v>
@@ -9438,7 +9435,7 @@
         <v>2</v>
       </c>
       <c r="C506" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D506" s="1" t="s">
         <v>13</v>
@@ -10180,7 +10177,7 @@
         <v>2</v>
       </c>
       <c r="C559" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D559" s="1" t="s">
         <v>13</v>
@@ -10516,7 +10513,7 @@
         <v>2</v>
       </c>
       <c r="C583" s="1" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
       <c r="D583" s="1" t="s">
         <v>13</v>
@@ -10600,7 +10597,7 @@
         <v>2</v>
       </c>
       <c r="C589" s="1" t="s">
-        <v>118</v>
+        <v>5</v>
       </c>
       <c r="D589" s="1" t="s">
         <v>13</v>
@@ -10723,27 +10720,27 @@
         <v>610</v>
       </c>
       <c r="B598" s="1" t="n">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="C598" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D598" s="1" t="s">
-        <v>13</v>
+        <v>611</v>
       </c>
     </row>
     <row r="599" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A599" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="B599" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="C599" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D599" s="1" t="s">
         <v>611</v>
-      </c>
-      <c r="B599" s="1" t="n">
-        <v>35</v>
-      </c>
-      <c r="C599" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D599" s="1" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="600" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10751,13 +10748,13 @@
         <v>613</v>
       </c>
       <c r="B600" s="1" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C600" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D600" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="601" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10765,13 +10762,13 @@
         <v>614</v>
       </c>
       <c r="B601" s="1" t="n">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C601" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D601" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="602" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10779,13 +10776,13 @@
         <v>615</v>
       </c>
       <c r="B602" s="1" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C602" s="1" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D602" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="603" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10793,13 +10790,13 @@
         <v>616</v>
       </c>
       <c r="B603" s="1" t="n">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C603" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D603" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="604" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10813,7 +10810,7 @@
         <v>13</v>
       </c>
       <c r="D604" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="605" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10821,13 +10818,13 @@
         <v>618</v>
       </c>
       <c r="B605" s="1" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C605" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D605" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="606" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10835,13 +10832,13 @@
         <v>619</v>
       </c>
       <c r="B606" s="1" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C606" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D606" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="607" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10849,13 +10846,13 @@
         <v>620</v>
       </c>
       <c r="B607" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C607" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D607" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="608" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10866,10 +10863,10 @@
         <v>8</v>
       </c>
       <c r="C608" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D608" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="609" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10883,7 +10880,7 @@
         <v>8</v>
       </c>
       <c r="D609" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="610" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10891,13 +10888,13 @@
         <v>623</v>
       </c>
       <c r="B610" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C610" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D610" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="611" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10905,13 +10902,13 @@
         <v>624</v>
       </c>
       <c r="B611" s="1" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C611" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D611" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="612" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10925,7 +10922,7 @@
         <v>13</v>
       </c>
       <c r="D612" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="613" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10939,7 +10936,7 @@
         <v>13</v>
       </c>
       <c r="D613" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="614" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10950,10 +10947,10 @@
         <v>5</v>
       </c>
       <c r="C614" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D614" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="615" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10961,13 +10958,13 @@
         <v>628</v>
       </c>
       <c r="B615" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C615" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D615" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="616" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10975,13 +10972,13 @@
         <v>629</v>
       </c>
       <c r="B616" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C616" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D616" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="617" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10995,7 +10992,7 @@
         <v>13</v>
       </c>
       <c r="D617" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="618" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11009,7 +11006,7 @@
         <v>13</v>
       </c>
       <c r="D618" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="619" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11023,7 +11020,7 @@
         <v>13</v>
       </c>
       <c r="D619" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="620" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11034,10 +11031,10 @@
         <v>3</v>
       </c>
       <c r="C620" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D620" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="621" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11051,7 +11048,7 @@
         <v>8</v>
       </c>
       <c r="D621" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="622" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11065,7 +11062,7 @@
         <v>8</v>
       </c>
       <c r="D622" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="623" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11076,10 +11073,10 @@
         <v>3</v>
       </c>
       <c r="C623" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D623" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="624" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11093,7 +11090,7 @@
         <v>19</v>
       </c>
       <c r="D624" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="625" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11104,10 +11101,10 @@
         <v>3</v>
       </c>
       <c r="C625" s="1" t="s">
-        <v>19</v>
+        <v>118</v>
       </c>
       <c r="D625" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="626" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11115,13 +11112,13 @@
         <v>639</v>
       </c>
       <c r="B626" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C626" s="1" t="s">
-        <v>118</v>
+        <v>13</v>
       </c>
       <c r="D626" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="627" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11135,7 +11132,7 @@
         <v>13</v>
       </c>
       <c r="D627" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="628" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11149,7 +11146,7 @@
         <v>13</v>
       </c>
       <c r="D628" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="629" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11163,7 +11160,7 @@
         <v>13</v>
       </c>
       <c r="D629" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="630" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11177,7 +11174,7 @@
         <v>13</v>
       </c>
       <c r="D630" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="631" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11188,10 +11185,10 @@
         <v>2</v>
       </c>
       <c r="C631" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D631" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="632" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11205,7 +11202,7 @@
         <v>8</v>
       </c>
       <c r="D632" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="633" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11219,7 +11216,7 @@
         <v>8</v>
       </c>
       <c r="D633" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="634" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11233,7 +11230,7 @@
         <v>8</v>
       </c>
       <c r="D634" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="635" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11247,7 +11244,7 @@
         <v>8</v>
       </c>
       <c r="D635" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="636" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11258,10 +11255,10 @@
         <v>2</v>
       </c>
       <c r="C636" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D636" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="637" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11275,7 +11272,7 @@
         <v>19</v>
       </c>
       <c r="D637" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="638" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11283,27 +11280,27 @@
         <v>651</v>
       </c>
       <c r="B638" s="1" t="n">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="C638" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D638" s="1" t="s">
-        <v>612</v>
+        <v>652</v>
       </c>
     </row>
     <row r="639" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A639" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="B639" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="C639" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D639" s="1" t="s">
         <v>652</v>
-      </c>
-      <c r="B639" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="C639" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D639" s="1" t="s">
-        <v>653</v>
       </c>
     </row>
     <row r="640" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11311,13 +11308,13 @@
         <v>654</v>
       </c>
       <c r="B640" s="1" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C640" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D640" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="641" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11325,13 +11322,13 @@
         <v>655</v>
       </c>
       <c r="B641" s="1" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C641" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D641" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="642" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11339,13 +11336,13 @@
         <v>656</v>
       </c>
       <c r="B642" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C642" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D642" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="643" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11353,13 +11350,13 @@
         <v>657</v>
       </c>
       <c r="B643" s="1" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C643" s="1" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D643" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="644" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11367,13 +11364,13 @@
         <v>658</v>
       </c>
       <c r="B644" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C644" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D644" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="645" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11381,13 +11378,13 @@
         <v>659</v>
       </c>
       <c r="B645" s="1" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C645" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D645" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="646" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11401,7 +11398,7 @@
         <v>13</v>
       </c>
       <c r="D646" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="647" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11409,13 +11406,13 @@
         <v>661</v>
       </c>
       <c r="B647" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C647" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D647" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="648" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11423,13 +11420,13 @@
         <v>662</v>
       </c>
       <c r="B648" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C648" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D648" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="649" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11443,7 +11440,7 @@
         <v>13</v>
       </c>
       <c r="D649" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="650" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11457,7 +11454,7 @@
         <v>13</v>
       </c>
       <c r="D650" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="651" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11468,10 +11465,10 @@
         <v>4</v>
       </c>
       <c r="C651" s="1" t="s">
-        <v>13</v>
+        <v>118</v>
       </c>
       <c r="D651" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="652" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11479,13 +11476,13 @@
         <v>666</v>
       </c>
       <c r="B652" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C652" s="1" t="s">
-        <v>118</v>
+        <v>13</v>
       </c>
       <c r="D652" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="653" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11496,10 +11493,10 @@
         <v>3</v>
       </c>
       <c r="C653" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D653" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="654" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11510,10 +11507,10 @@
         <v>3</v>
       </c>
       <c r="C654" s="1" t="s">
-        <v>8</v>
+        <v>118</v>
       </c>
       <c r="D654" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="655" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11524,10 +11521,10 @@
         <v>3</v>
       </c>
       <c r="C655" s="1" t="s">
-        <v>118</v>
+        <v>5</v>
       </c>
       <c r="D655" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="656" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11535,13 +11532,13 @@
         <v>670</v>
       </c>
       <c r="B656" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C656" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D656" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="657" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11555,7 +11552,7 @@
         <v>13</v>
       </c>
       <c r="D657" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="658" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11569,7 +11566,7 @@
         <v>13</v>
       </c>
       <c r="D658" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="659" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11583,7 +11580,7 @@
         <v>13</v>
       </c>
       <c r="D659" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="660" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11597,7 +11594,7 @@
         <v>13</v>
       </c>
       <c r="D660" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="661" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11611,7 +11608,7 @@
         <v>13</v>
       </c>
       <c r="D661" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="662" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11625,7 +11622,7 @@
         <v>13</v>
       </c>
       <c r="D662" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="663" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11639,7 +11636,7 @@
         <v>13</v>
       </c>
       <c r="D663" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="664" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11653,7 +11650,7 @@
         <v>13</v>
       </c>
       <c r="D664" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="665" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11664,10 +11661,10 @@
         <v>2</v>
       </c>
       <c r="C665" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D665" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="666" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11678,10 +11675,10 @@
         <v>2</v>
       </c>
       <c r="C666" s="1" t="s">
-        <v>8</v>
+        <v>118</v>
       </c>
       <c r="D666" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="667" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11692,10 +11689,10 @@
         <v>2</v>
       </c>
       <c r="C667" s="1" t="s">
-        <v>118</v>
+        <v>5</v>
       </c>
       <c r="D667" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="668" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11709,7 +11706,7 @@
         <v>5</v>
       </c>
       <c r="D668" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="669" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11717,27 +11714,27 @@
         <v>683</v>
       </c>
       <c r="B669" s="1" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C669" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D669" s="1" t="s">
-        <v>653</v>
+        <v>684</v>
       </c>
     </row>
     <row r="670" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A670" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="B670" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="C670" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D670" s="1" t="s">
         <v>684</v>
-      </c>
-      <c r="B670" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="C670" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D670" s="1" t="s">
-        <v>685</v>
       </c>
     </row>
     <row r="671" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11745,13 +11742,13 @@
         <v>686</v>
       </c>
       <c r="B671" s="1" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C671" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D671" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="672" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11759,13 +11756,13 @@
         <v>687</v>
       </c>
       <c r="B672" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="C672" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C672" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D672" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="673" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11773,13 +11770,13 @@
         <v>688</v>
       </c>
       <c r="B673" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C673" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D673" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="674" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11793,7 +11790,7 @@
         <v>13</v>
       </c>
       <c r="D674" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="675" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11801,13 +11798,13 @@
         <v>690</v>
       </c>
       <c r="B675" s="1" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C675" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D675" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="676" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11821,7 +11818,7 @@
         <v>13</v>
       </c>
       <c r="D676" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="677" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11835,7 +11832,7 @@
         <v>13</v>
       </c>
       <c r="D677" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="678" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11849,7 +11846,7 @@
         <v>13</v>
       </c>
       <c r="D678" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="679" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11863,7 +11860,7 @@
         <v>13</v>
       </c>
       <c r="D679" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="680" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11874,10 +11871,10 @@
         <v>2</v>
       </c>
       <c r="C680" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D680" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="681" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11891,7 +11888,7 @@
         <v>8</v>
       </c>
       <c r="D681" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="682" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11899,27 +11896,27 @@
         <v>697</v>
       </c>
       <c r="B682" s="1" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="C682" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D682" s="1" t="s">
-        <v>685</v>
+        <v>698</v>
       </c>
     </row>
     <row r="683" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A683" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="B683" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="C683" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D683" s="1" t="s">
         <v>698</v>
-      </c>
-      <c r="B683" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="C683" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D683" s="1" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="684" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11933,7 +11930,7 @@
         <v>13</v>
       </c>
       <c r="D684" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="685" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11941,13 +11938,13 @@
         <v>701</v>
       </c>
       <c r="B685" s="1" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C685" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D685" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="686" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11961,7 +11958,7 @@
         <v>13</v>
       </c>
       <c r="D686" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="687" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11969,27 +11966,27 @@
         <v>703</v>
       </c>
       <c r="B687" s="1" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="C687" s="1" t="s">
-        <v>13</v>
+        <v>704</v>
       </c>
       <c r="D687" s="1" t="s">
-        <v>699</v>
+        <v>705</v>
       </c>
     </row>
     <row r="688" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A688" s="1" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="B688" s="1" t="n">
         <v>19</v>
       </c>
       <c r="C688" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="D688" s="1" t="s">
         <v>705</v>
-      </c>
-      <c r="D688" s="1" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="689" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11997,13 +11994,13 @@
         <v>707</v>
       </c>
       <c r="B689" s="1" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C689" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="D689" s="1" t="s">
         <v>705</v>
-      </c>
-      <c r="D689" s="1" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="690" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12011,13 +12008,13 @@
         <v>708</v>
       </c>
       <c r="B690" s="1" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C690" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="D690" s="1" t="s">
         <v>705</v>
-      </c>
-      <c r="D690" s="1" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="691" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12025,13 +12022,13 @@
         <v>709</v>
       </c>
       <c r="B691" s="1" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C691" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D691" s="1" t="s">
         <v>705</v>
-      </c>
-      <c r="D691" s="1" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="692" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12039,13 +12036,13 @@
         <v>710</v>
       </c>
       <c r="B692" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C692" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D692" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="693" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12053,13 +12050,13 @@
         <v>711</v>
       </c>
       <c r="B693" s="1" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C693" s="1" t="s">
-        <v>13</v>
+        <v>704</v>
       </c>
       <c r="D693" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
     <row r="694" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12070,10 +12067,10 @@
         <v>2</v>
       </c>
       <c r="C694" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="D694" s="1" t="s">
         <v>705</v>
-      </c>
-      <c r="D694" s="1" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="695" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12084,10 +12081,10 @@
         <v>2</v>
       </c>
       <c r="C695" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D695" s="1" t="s">
         <v>705</v>
-      </c>
-      <c r="D695" s="1" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="696" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12101,21 +12098,7 @@
         <v>13</v>
       </c>
       <c r="D696" s="1" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="697" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A697" s="1" t="s">
-        <v>715</v>
-      </c>
-      <c r="B697" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C697" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D697" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
     </row>
   </sheetData>

</xml_diff>